<commit_message>
Changes to production plan
</commit_message>
<xml_diff>
--- a/Skeleton_Party_production_plan.xlsx
+++ b/Skeleton_Party_production_plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazzt\Documents\GitHub\Skeleton-Party\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\Documents\GitHub\Skeleton-Party\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C788CDA-4739-480E-A6B7-AC814FD33ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CAC3DD-C329-4189-96B3-FE0CEEE1CB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="9" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="203">
   <si>
     <t>TASK</t>
   </si>
@@ -975,6 +975,9 @@
   <si>
     <t>Mage's explosion attack with all skills tree features implemented</t>
   </si>
+  <si>
+    <t>Update Main Menu Design</t>
+  </si>
 </sst>
 </file>
 
@@ -1774,7 +1777,10 @@
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="198">
+  <dxfs count="199">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1816,6 +1822,94 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2520,6 +2614,14 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode=";;;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
@@ -3166,6 +3268,27 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -3185,118 +3308,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3396,7 +3407,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74B39E37-C695-4FB4-9659-696DC3C4B7D6}" name="Table1" displayName="Table1" ref="A8:R16" totalsRowShown="0" headerRowDxfId="197">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74B39E37-C695-4FB4-9659-696DC3C4B7D6}" name="Table1" displayName="Table1" ref="A8:R16" totalsRowShown="0" headerRowDxfId="195">
   <autoFilter ref="A8:R16" xr:uid="{74B39E37-C695-4FB4-9659-696DC3C4B7D6}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{3AB7DF63-F3E2-46EA-867C-B10FAF5F8283}" name="Student Name"/>
@@ -3406,16 +3417,16 @@
     <tableColumn id="5" xr3:uid="{2BA79B57-539F-46E5-965A-5E7716ACBE1C}" name="In Progress"/>
     <tableColumn id="6" xr3:uid="{2710B94F-2F91-48AC-8457-97A764EF4BC7}" name="Not Started"/>
     <tableColumn id="7" xr3:uid="{493E51FB-9F1A-4B86-B51A-0A9F697471BC}" name="Total Workload "/>
-    <tableColumn id="8" xr3:uid="{B5D3A34D-58ED-4437-86C3-EDEF21DC68ED}" name="Planned Code %" dataDxfId="196"/>
-    <tableColumn id="9" xr3:uid="{91977D25-FF71-40D1-8F42-2C68A990D6AF}" name="Workload" dataDxfId="195"/>
+    <tableColumn id="8" xr3:uid="{B5D3A34D-58ED-4437-86C3-EDEF21DC68ED}" name="Planned Code %" dataDxfId="194"/>
+    <tableColumn id="9" xr3:uid="{91977D25-FF71-40D1-8F42-2C68A990D6AF}" name="Workload" dataDxfId="193"/>
     <tableColumn id="10" xr3:uid="{20ECF3E5-B447-40AE-82D9-F1DAECBAD66F}" name="Remaining"/>
-    <tableColumn id="11" xr3:uid="{86055431-90BE-4435-8CF6-21581B8D435B}" name="Workload2" dataDxfId="194"/>
+    <tableColumn id="11" xr3:uid="{86055431-90BE-4435-8CF6-21581B8D435B}" name="Workload2" dataDxfId="192"/>
     <tableColumn id="12" xr3:uid="{5AA91C7C-8A0B-454F-BB15-D1BB545F0BE4}" name="Remaining3"/>
-    <tableColumn id="13" xr3:uid="{55A241A8-0143-4DEA-8DFD-95E60EC7AFD6}" name="Workload4" dataDxfId="193"/>
+    <tableColumn id="13" xr3:uid="{55A241A8-0143-4DEA-8DFD-95E60EC7AFD6}" name="Workload4" dataDxfId="191"/>
     <tableColumn id="14" xr3:uid="{B367E59C-5FB9-479C-A7F3-B1C7AE02BA4A}" name="Remaining5"/>
-    <tableColumn id="15" xr3:uid="{57F47D13-B340-4FE1-8235-443CABD5B1EA}" name="Workload6" dataDxfId="192"/>
+    <tableColumn id="15" xr3:uid="{57F47D13-B340-4FE1-8235-443CABD5B1EA}" name="Workload6" dataDxfId="190"/>
     <tableColumn id="16" xr3:uid="{DF492611-AC03-4727-883A-97854465FDAE}" name="Remaining7"/>
-    <tableColumn id="17" xr3:uid="{9A20AE32-79C9-4662-A53C-09867FD35D7D}" name="Workload8" dataDxfId="191"/>
+    <tableColumn id="17" xr3:uid="{9A20AE32-79C9-4662-A53C-09867FD35D7D}" name="Workload8" dataDxfId="189"/>
     <tableColumn id="18" xr3:uid="{67CDA12C-F1E4-40F4-B6AC-BDC17A0B0B8D}" name="Remaining9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3434,11 +3445,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C73C9A4E-E4B8-40B0-BB86-7BA7DB9B8E56}" name="Table4" displayName="Table4" ref="A5:B8" totalsRowShown="0" headerRowDxfId="190" headerRowBorderDxfId="189" tableBorderDxfId="188" totalsRowBorderDxfId="187">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C73C9A4E-E4B8-40B0-BB86-7BA7DB9B8E56}" name="Table4" displayName="Table4" ref="A5:B8" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A5:B8" xr:uid="{C73C9A4E-E4B8-40B0-BB86-7BA7DB9B8E56}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{72CD6C81-E3FF-479B-8443-C59651900B72}" name="Status" dataDxfId="186"/>
-    <tableColumn id="2" xr3:uid="{B1C91A3B-EB58-4009-B130-F6CBDA1769C2}" name="Description" dataDxfId="185"/>
+    <tableColumn id="1" xr3:uid="{72CD6C81-E3FF-479B-8443-C59651900B72}" name="Status" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B1C91A3B-EB58-4009-B130-F6CBDA1769C2}" name="Description" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3449,7 +3460,7 @@
   <autoFilter ref="A1:B4" xr:uid="{DECAA8B5-6330-451B-9562-5424BBB00F80}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D55844DA-51EF-4755-A498-8AFCDF33F45D}" name="Colour"/>
-    <tableColumn id="2" xr3:uid="{B0848137-1086-4330-AA22-48E2FA796BAF}" name="Description" dataDxfId="184"/>
+    <tableColumn id="2" xr3:uid="{B0848137-1086-4330-AA22-48E2FA796BAF}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4195,11 +4206,11 @@
       </c>
       <c r="E13">
         <f>SUMIFS(GANTT!F:F, GANTT!G:G, Main!$A13, GANTT!R:R,TaskStatus!$A$7)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F13">
         <f>SUMIFS(GANTT!F:F, GANTT!G:G, Main!$A13, GANTT!R:R,TaskStatus!$A$6)</f>
-        <v>34.5</v>
+        <v>14.5</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -4383,11 +4394,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -4454,13 +4465,13 @@
     <mergeCell ref="O7:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="183" priority="1" operator="containsText" text="GREEN">
+    <cfRule type="containsText" dxfId="198" priority="1" operator="containsText" text="GREEN">
       <formula>NOT(ISERROR(SEARCH("GREEN",B5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="2" operator="containsText" text="YELLOW">
+    <cfRule type="containsText" dxfId="197" priority="2" operator="containsText" text="YELLOW">
       <formula>NOT(ISERROR(SEARCH("YELLOW",B5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="3" operator="containsText" text="RED">
+    <cfRule type="containsText" dxfId="196" priority="3" operator="containsText" text="RED">
       <formula>NOT(ISERROR(SEARCH("RED",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4486,24 +4497,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BZ115"/>
+  <dimension ref="A1:BZ116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="18" ySplit="7" topLeftCell="S8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane xSplit="18" ySplit="7" topLeftCell="S17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="22" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="14.33203125" style="22" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="245.5546875" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="20.88671875" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="22" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="14.33203125" style="22" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="245.5546875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="20.88671875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="22.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17.6640625" style="54" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.44140625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -5804,7 +5815,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="70">
-        <f t="shared" ref="J13:J87" si="13">H13 +I13</f>
+        <f t="shared" ref="J13:J88" si="13">H13 +I13</f>
         <v>44496</v>
       </c>
       <c r="K13" s="72" t="s">
@@ -5822,7 +5833,7 @@
         <v>2</v>
       </c>
       <c r="P13" s="70">
-        <f t="shared" ref="P13:P87" si="14">N13+O13</f>
+        <f t="shared" ref="P13:P88" si="14">N13+O13</f>
         <v>44496</v>
       </c>
       <c r="Q13" s="69">
@@ -7376,12 +7387,18 @@
       <c r="K22" s="74"/>
       <c r="L22" s="74"/>
       <c r="M22" s="74"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="76"/>
+      <c r="N22" s="75">
+        <v>44506</v>
+      </c>
+      <c r="O22" s="76">
+        <v>1</v>
+      </c>
       <c r="P22" s="75"/>
-      <c r="Q22" s="74"/>
+      <c r="Q22" s="74">
+        <v>5</v>
+      </c>
       <c r="R22" s="74" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S22" s="16"/>
       <c r="T22" s="16"/>
@@ -7462,12 +7479,18 @@
         <v>#N/A</v>
       </c>
       <c r="M23" s="74"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="76"/>
+      <c r="N23" s="75">
+        <v>44507</v>
+      </c>
+      <c r="O23" s="76">
+        <v>1</v>
+      </c>
       <c r="P23" s="75"/>
-      <c r="Q23" s="74"/>
+      <c r="Q23" s="74">
+        <v>5</v>
+      </c>
       <c r="R23" s="74" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S23" s="16">
         <f t="shared" si="8"/>
@@ -7523,7 +7546,7 @@
       </c>
       <c r="AF23" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG23" s="16">
         <f t="shared" si="9"/>
@@ -8184,7 +8207,7 @@
         <v>56</v>
       </c>
       <c r="S27" s="16" t="e">
-        <f t="shared" ref="S27:AB41" si="15">IF(AND(S$6&gt;=$N27,S$6&lt;$N27+$O27), 1, IF(AND(S$6&gt;=$H27,S$6&lt;$H27+$I27), 2, 0))</f>
+        <f t="shared" ref="S27:AB42" si="15">IF(AND(S$6&gt;=$N27,S$6&lt;$N27+$O27), 1, IF(AND(S$6&gt;=$H27,S$6&lt;$H27+$I27), 2, 0))</f>
         <v>#VALUE!</v>
       </c>
       <c r="T27" s="16" t="e">
@@ -8224,7 +8247,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AC27" s="16" t="e">
-        <f t="shared" ref="AC27:AL41" si="16">IF(AND(AC$6&gt;=$N27,AC$6&lt;$N27+$O27), 1, IF(AND(AC$6&gt;=$H27,AC$6&lt;$H27+$I27), 2, 0))</f>
+        <f t="shared" ref="AC27:AL42" si="16">IF(AND(AC$6&gt;=$N27,AC$6&lt;$N27+$O27), 1, IF(AND(AC$6&gt;=$H27,AC$6&lt;$H27+$I27), 2, 0))</f>
         <v>#VALUE!</v>
       </c>
       <c r="AD27" s="16" t="e">
@@ -8264,7 +8287,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AM27" s="16" t="e">
-        <f t="shared" ref="AM27:AV41" si="17">IF(AND(AM$6&gt;=$N27,AM$6&lt;$N27+$O27), 1, IF(AND(AM$6&gt;=$H27,AM$6&lt;$H27+$I27), 2, 0))</f>
+        <f t="shared" ref="AM27:AV42" si="17">IF(AND(AM$6&gt;=$N27,AM$6&lt;$N27+$O27), 1, IF(AND(AM$6&gt;=$H27,AM$6&lt;$H27+$I27), 2, 0))</f>
         <v>#VALUE!</v>
       </c>
       <c r="AN27" s="16" t="e">
@@ -8304,7 +8327,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AW27" s="16" t="e">
-        <f t="shared" ref="AW27:BF41" si="18">IF(AND(AW$6&gt;=$N27,AW$6&lt;$N27+$O27), 1, IF(AND(AW$6&gt;=$H27,AW$6&lt;$H27+$I27), 2, 0))</f>
+        <f t="shared" ref="AW27:BF42" si="18">IF(AND(AW$6&gt;=$N27,AW$6&lt;$N27+$O27), 1, IF(AND(AW$6&gt;=$H27,AW$6&lt;$H27+$I27), 2, 0))</f>
         <v>#VALUE!</v>
       </c>
       <c r="AX27" s="16" t="e">
@@ -8344,7 +8367,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="BG27" s="16" t="e">
-        <f t="shared" ref="BG27:BH41" si="19">IF(AND(BG$6&gt;=$N27,BG$6&lt;$N27+$O27), 1, IF(AND(BG$6&gt;=$H27,BG$6&lt;$H27+$I27), 2, 0))</f>
+        <f t="shared" ref="BG27:BH42" si="19">IF(AND(BG$6&gt;=$N27,BG$6&lt;$N27+$O27), 1, IF(AND(BG$6&gt;=$H27,BG$6&lt;$H27+$I27), 2, 0))</f>
         <v>#VALUE!</v>
       </c>
       <c r="BH27" s="16" t="e">
@@ -9178,12 +9201,18 @@
       <c r="K34" s="74"/>
       <c r="L34" s="74"/>
       <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76"/>
+      <c r="N34" s="75">
+        <v>44514</v>
+      </c>
+      <c r="O34" s="76">
+        <v>1</v>
+      </c>
       <c r="P34" s="75"/>
-      <c r="Q34" s="74"/>
+      <c r="Q34" s="74">
+        <v>5</v>
+      </c>
       <c r="R34" s="74" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
@@ -9228,238 +9257,115 @@
       <c r="BG34" s="16"/>
       <c r="BH34" s="16"/>
     </row>
-    <row r="35" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="82" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="F35" s="66">
-        <v>1.5</v>
-      </c>
+    <row r="35" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="74" t="s">
         <v>105</v>
       </c>
       <c r="H35" s="75">
-        <v>44512</v>
+        <v>44508</v>
       </c>
       <c r="I35" s="74">
         <v>1</v>
       </c>
-      <c r="J35" s="75">
+      <c r="J35" s="75"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="75">
+        <v>44513</v>
+      </c>
+      <c r="O35" s="76">
+        <v>1</v>
+      </c>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="74">
+        <v>5</v>
+      </c>
+      <c r="R35" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="16"/>
+      <c r="AH35" s="16"/>
+      <c r="AI35" s="16"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="16"/>
+      <c r="AM35" s="16"/>
+      <c r="AN35" s="16"/>
+      <c r="AO35" s="16"/>
+      <c r="AP35" s="16"/>
+      <c r="AQ35" s="16"/>
+      <c r="AR35" s="16"/>
+      <c r="AS35" s="16"/>
+      <c r="AT35" s="16"/>
+      <c r="AU35" s="16"/>
+      <c r="AV35" s="16"/>
+      <c r="AW35" s="16"/>
+      <c r="AX35" s="16"/>
+      <c r="AY35" s="16"/>
+      <c r="AZ35" s="16"/>
+      <c r="BA35" s="16"/>
+      <c r="BB35" s="16"/>
+      <c r="BC35" s="16"/>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="16"/>
+      <c r="BG35" s="16"/>
+      <c r="BH35" s="16"/>
+    </row>
+    <row r="36" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="64" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" s="66">
+        <v>1.5</v>
+      </c>
+      <c r="G36" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36" s="75">
+        <v>44512</v>
+      </c>
+      <c r="I36" s="74">
+        <v>1</v>
+      </c>
+      <c r="J36" s="75">
         <f t="shared" si="13"/>
         <v>44513</v>
-      </c>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74" t="e">
-        <f>LOOKUP(K35,TaskGrading!$A$4:$A$7,TaskGrading!$C$4:$C$7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M35" s="74"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="75">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="S35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="T35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="U35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="V35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="W35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="X35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="Y35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="Z35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AA35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AB35" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AC35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AD35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AE35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AF35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AG35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AH35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AI35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AJ35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AK35" s="16">
-        <f t="shared" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="AL35" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AM35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AN35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AO35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AP35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AQ35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AR35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AS35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AT35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AU35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AV35" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AW35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AX35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AY35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AZ35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BA35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BB35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BC35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BD35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BE35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BF35" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="BG35" s="16">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="BH35" s="16">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="75">
-        <f t="shared" si="13"/>
-        <v>0</v>
       </c>
       <c r="K36" s="74"/>
       <c r="L36" s="74" t="e">
@@ -9467,14 +9373,16 @@
         <v>#N/A</v>
       </c>
       <c r="M36" s="74"/>
-      <c r="N36" s="74"/>
+      <c r="N36" s="75"/>
       <c r="O36" s="76"/>
       <c r="P36" s="75">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q36" s="74"/>
-      <c r="R36" s="74"/>
+      <c r="R36" s="74" t="s">
+        <v>56</v>
+      </c>
       <c r="S36" s="16">
         <f t="shared" si="15"/>
         <v>0</v>
@@ -9549,7 +9457,7 @@
       </c>
       <c r="AK36" s="16">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL36" s="16">
         <f t="shared" si="16"/>
@@ -9644,33 +9552,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>75</v>
-      </c>
+    <row r="37" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="82"/>
       <c r="E37" s="14"/>
-      <c r="F37" s="66">
-        <v>1</v>
-      </c>
-      <c r="G37" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="H37" s="75">
-        <v>44515</v>
-      </c>
-      <c r="I37" s="74">
-        <v>3</v>
-      </c>
+      <c r="F37" s="66"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="74"/>
       <c r="J37" s="75">
         <f t="shared" si="13"/>
-        <v>44518</v>
+        <v>0</v>
       </c>
       <c r="K37" s="74"/>
       <c r="L37" s="74" t="e">
@@ -9685,9 +9581,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="74"/>
-      <c r="R37" s="74" t="s">
-        <v>56</v>
-      </c>
+      <c r="R37" s="74"/>
       <c r="S37" s="16">
         <f t="shared" si="15"/>
         <v>0</v>
@@ -9774,15 +9668,15 @@
       </c>
       <c r="AN37" s="16">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO37" s="16">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP37" s="16">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ37" s="16">
         <f t="shared" si="17"/>
@@ -9859,13 +9753,13 @@
     </row>
     <row r="38" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D38" s="82"/>
       <c r="E38" s="14"/>
@@ -9873,17 +9767,17 @@
         <v>1</v>
       </c>
       <c r="G38" s="74" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H38" s="75">
         <v>44515</v>
       </c>
       <c r="I38" s="74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J38" s="75">
         <f t="shared" si="13"/>
-        <v>44516</v>
+        <v>44518</v>
       </c>
       <c r="K38" s="74"/>
       <c r="L38" s="74" t="e">
@@ -9991,11 +9885,11 @@
       </c>
       <c r="AO38" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP38" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ38" s="16">
         <f t="shared" si="17"/>
@@ -10072,31 +9966,31 @@
     </row>
     <row r="39" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D39" s="82"/>
       <c r="E39" s="14"/>
       <c r="F39" s="66">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G39" s="74" t="s">
         <v>99</v>
       </c>
       <c r="H39" s="75">
-        <v>44548</v>
+        <v>44515</v>
       </c>
       <c r="I39" s="74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" s="75">
         <f t="shared" si="13"/>
-        <v>44550</v>
+        <v>44516</v>
       </c>
       <c r="K39" s="74"/>
       <c r="L39" s="74" t="e">
@@ -10200,7 +10094,7 @@
       </c>
       <c r="AN39" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO39" s="16">
         <f t="shared" si="17"/>
@@ -10285,7 +10179,7 @@
     </row>
     <row r="40" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>19</v>
@@ -10299,17 +10193,17 @@
         <v>4</v>
       </c>
       <c r="G40" s="74" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H40" s="75">
-        <v>44515</v>
+        <v>44548</v>
       </c>
       <c r="I40" s="74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J40" s="75">
         <f t="shared" si="13"/>
-        <v>44518</v>
+        <v>44550</v>
       </c>
       <c r="K40" s="74"/>
       <c r="L40" s="74" t="e">
@@ -10413,15 +10307,15 @@
       </c>
       <c r="AN40" s="16">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO40" s="16">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP40" s="16">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ40" s="16">
         <f t="shared" si="17"/>
@@ -10498,10 +10392,10 @@
     </row>
     <row r="41" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>77</v>
@@ -10512,17 +10406,17 @@
         <v>4</v>
       </c>
       <c r="G41" s="74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H41" s="75">
         <v>44515</v>
       </c>
       <c r="I41" s="74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J41" s="75">
         <f t="shared" si="13"/>
-        <v>44516</v>
+        <v>44518</v>
       </c>
       <c r="K41" s="74"/>
       <c r="L41" s="74" t="e">
@@ -10630,11 +10524,11 @@
       </c>
       <c r="AO41" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP41" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ41" s="16">
         <f t="shared" si="17"/>
@@ -10711,7 +10605,7 @@
     </row>
     <row r="42" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B42" s="26" t="s">
         <v>20</v>
@@ -10728,14 +10622,14 @@
         <v>103</v>
       </c>
       <c r="H42" s="75">
-        <v>44548</v>
+        <v>44515</v>
       </c>
       <c r="I42" s="74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J42" s="75">
         <f t="shared" si="13"/>
-        <v>44550</v>
+        <v>44516</v>
       </c>
       <c r="K42" s="74"/>
       <c r="L42" s="74" t="e">
@@ -10754,201 +10648,201 @@
         <v>56</v>
       </c>
       <c r="S42" s="16">
-        <f t="shared" ref="S42:AB51" si="20">IF(AND(S$6&gt;=$N42,S$6&lt;$N42+$O42), 1, IF(AND(S$6&gt;=$H42,S$6&lt;$H42+$I42), 2, 0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="U42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Z42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AA42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB42" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AC42" s="16">
-        <f t="shared" ref="AC42:AL51" si="21">IF(AND(AC$6&gt;=$N42,AC$6&lt;$N42+$O42), 1, IF(AND(AC$6&gt;=$H42,AC$6&lt;$H42+$I42), 2, 0))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AH42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AI42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AJ42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AK42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL42" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AM42" s="16">
-        <f t="shared" ref="AM42:AV51" si="22">IF(AND(AM$6&gt;=$N42,AM$6&lt;$N42+$O42), 1, IF(AND(AM$6&gt;=$H42,AM$6&lt;$H42+$I42), 2, 0))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AN42" s="16">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>2</v>
       </c>
       <c r="AO42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AP42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AQ42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AR42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AS42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AT42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AU42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AV42" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AW42" s="16">
-        <f t="shared" ref="AW42:BF51" si="23">IF(AND(AW$6&gt;=$N42,AW$6&lt;$N42+$O42), 1, IF(AND(AW$6&gt;=$H42,AW$6&lt;$H42+$I42), 2, 0))</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AX42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AY42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AZ42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BA42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BB42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BC42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BD42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BE42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BF42" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BG42" s="16">
-        <f t="shared" ref="BG42:BH51" si="24">IF(AND(BG$6&gt;=$N42,BG$6&lt;$N42+$O42), 1, IF(AND(BG$6&gt;=$H42,BG$6&lt;$H42+$I42), 2, 0))</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="BH42" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="64" t="s">
-        <v>140</v>
+    <row r="43" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="65" t="s">
+        <v>139</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D43" s="82"/>
       <c r="E43" s="14"/>
       <c r="F43" s="66">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G43" s="74" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H43" s="75">
-        <v>44515</v>
+        <v>44548</v>
       </c>
       <c r="I43" s="74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J43" s="75">
         <f t="shared" si="13"/>
-        <v>44519</v>
+        <v>44550</v>
       </c>
       <c r="K43" s="74"/>
       <c r="L43" s="74" t="e">
@@ -10967,7 +10861,7 @@
         <v>56</v>
       </c>
       <c r="S43" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="S43:AB52" si="20">IF(AND(S$6&gt;=$N43,S$6&lt;$N43+$O43), 1, IF(AND(S$6&gt;=$H43,S$6&lt;$H43+$I43), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T43" s="16">
@@ -11007,7 +10901,7 @@
         <v>0</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="AC43:AL52" si="21">IF(AND(AC$6&gt;=$N43,AC$6&lt;$N43+$O43), 1, IF(AND(AC$6&gt;=$H43,AC$6&lt;$H43+$I43), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD43" s="16">
@@ -11047,24 +10941,24 @@
         <v>0</v>
       </c>
       <c r="AM43" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="AM43:AV52" si="22">IF(AND(AM$6&gt;=$N43,AM$6&lt;$N43+$O43), 1, IF(AND(AM$6&gt;=$H43,AM$6&lt;$H43+$I43), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN43" s="16">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO43" s="16">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP43" s="16">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ43" s="16">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR43" s="16">
         <f t="shared" si="22"/>
@@ -11087,7 +10981,7 @@
         <v>0</v>
       </c>
       <c r="AW43" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="AW43:BF52" si="23">IF(AND(AW$6&gt;=$N43,AW$6&lt;$N43+$O43), 1, IF(AND(AW$6&gt;=$H43,AW$6&lt;$H43+$I43), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX43" s="16">
@@ -11127,7 +11021,7 @@
         <v>0</v>
       </c>
       <c r="BG43" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="BG43:BH52" si="24">IF(AND(BG$6&gt;=$N43,BG$6&lt;$N43+$O43), 1, IF(AND(BG$6&gt;=$H43,BG$6&lt;$H43+$I43), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH43" s="16">
@@ -11136,20 +11030,32 @@
       </c>
     </row>
     <row r="44" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>76</v>
+      </c>
       <c r="D44" s="82"/>
       <c r="E44" s="14"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="74"/>
+      <c r="F44" s="66">
+        <v>1</v>
+      </c>
+      <c r="G44" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="75">
+        <v>44515</v>
+      </c>
+      <c r="I44" s="74">
+        <v>4</v>
+      </c>
       <c r="J44" s="75">
-        <f t="shared" ref="J44" si="25">H44 +I44</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>44519</v>
       </c>
       <c r="K44" s="74"/>
       <c r="L44" s="74" t="e">
@@ -11160,11 +11066,13 @@
       <c r="N44" s="74"/>
       <c r="O44" s="76"/>
       <c r="P44" s="75">
-        <f t="shared" ref="P44" si="26">N44+O44</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
+      <c r="R44" s="74" t="s">
+        <v>56</v>
+      </c>
       <c r="S44" s="16">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -11251,19 +11159,19 @@
       </c>
       <c r="AN44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR44" s="16">
         <f t="shared" si="22"/>
@@ -11334,33 +11242,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>75</v>
-      </c>
+    <row r="45" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="82"/>
       <c r="E45" s="14"/>
-      <c r="F45" s="66">
-        <v>8</v>
-      </c>
-      <c r="G45" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="H45" s="75">
-        <v>44522</v>
-      </c>
-      <c r="I45" s="74">
-        <v>2</v>
-      </c>
+      <c r="F45" s="66"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="75"/>
+      <c r="I45" s="74"/>
       <c r="J45" s="75">
-        <f t="shared" si="13"/>
-        <v>44524</v>
+        <f t="shared" ref="J45" si="25">H45 +I45</f>
+        <v>0</v>
       </c>
       <c r="K45" s="74"/>
       <c r="L45" s="74" t="e">
@@ -11371,13 +11267,11 @@
       <c r="N45" s="74"/>
       <c r="O45" s="76"/>
       <c r="P45" s="75">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="P45" si="26">N45+O45</f>
         <v>0</v>
       </c>
       <c r="Q45" s="74"/>
-      <c r="R45" s="74" t="s">
-        <v>56</v>
-      </c>
+      <c r="R45" s="74"/>
       <c r="S45" s="16">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -11492,11 +11386,11 @@
       </c>
       <c r="AU45" s="16">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AV45" s="16">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW45" s="16">
         <f t="shared" si="23"/>
@@ -11549,13 +11443,13 @@
     </row>
     <row r="46" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B46" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" s="82"/>
       <c r="E46" s="14"/>
@@ -11563,17 +11457,17 @@
         <v>8</v>
       </c>
       <c r="G46" s="74" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H46" s="75">
         <v>44522</v>
       </c>
       <c r="I46" s="74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J46" s="75">
         <f t="shared" si="13"/>
-        <v>44525</v>
+        <v>44524</v>
       </c>
       <c r="K46" s="74"/>
       <c r="L46" s="74" t="e">
@@ -11713,7 +11607,7 @@
       </c>
       <c r="AW46" s="16">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX46" s="16">
         <f t="shared" si="23"/>
@@ -11762,7 +11656,7 @@
     </row>
     <row r="47" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B47" s="26" t="s">
         <v>21</v>
@@ -11776,17 +11670,17 @@
         <v>8</v>
       </c>
       <c r="G47" s="74" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H47" s="75">
         <v>44522</v>
       </c>
       <c r="I47" s="74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J47" s="75">
         <f t="shared" si="13"/>
-        <v>44523</v>
+        <v>44525</v>
       </c>
       <c r="K47" s="74"/>
       <c r="L47" s="74" t="e">
@@ -11922,11 +11816,11 @@
       </c>
       <c r="AV47" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW47" s="16">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX47" s="16">
         <f t="shared" si="23"/>
@@ -11975,7 +11869,7 @@
     </row>
     <row r="48" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B48" s="26" t="s">
         <v>21</v>
@@ -11986,10 +11880,10 @@
       <c r="D48" s="82"/>
       <c r="E48" s="14"/>
       <c r="F48" s="66">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G48" s="74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" s="75">
         <v>44522</v>
@@ -12186,21 +12080,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="14"/>
+    <row r="49" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="82"/>
       <c r="E49" s="14"/>
-      <c r="F49" s="66"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="75"/>
-      <c r="I49" s="74"/>
+      <c r="F49" s="66">
+        <v>1</v>
+      </c>
+      <c r="G49" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="H49" s="75">
+        <v>44522</v>
+      </c>
+      <c r="I49" s="74">
+        <v>1</v>
+      </c>
       <c r="J49" s="75">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>44523</v>
       </c>
       <c r="K49" s="74"/>
       <c r="L49" s="74" t="e">
@@ -12215,7 +12121,9 @@
         <v>0</v>
       </c>
       <c r="Q49" s="74"/>
-      <c r="R49" s="74"/>
+      <c r="R49" s="74" t="s">
+        <v>56</v>
+      </c>
       <c r="S49" s="16">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -12330,7 +12238,7 @@
       </c>
       <c r="AU49" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV49" s="16">
         <f t="shared" si="22"/>
@@ -12385,33 +12293,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="39" t="s">
-        <v>77</v>
-      </c>
+    <row r="50" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="26"/>
+      <c r="C50" s="39"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
-      <c r="F50" s="66">
-        <v>4</v>
-      </c>
-      <c r="G50" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="H50" s="75">
-        <v>44529</v>
-      </c>
-      <c r="I50" s="74">
-        <v>4</v>
-      </c>
+      <c r="F50" s="66"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="74"/>
       <c r="J50" s="75">
         <f t="shared" si="13"/>
-        <v>44533</v>
+        <v>0</v>
       </c>
       <c r="K50" s="74"/>
       <c r="L50" s="74" t="e">
@@ -12426,9 +12322,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="74"/>
-      <c r="R50" s="74" t="s">
-        <v>56</v>
-      </c>
+      <c r="R50" s="74"/>
       <c r="S50" s="16">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -12571,19 +12465,19 @@
       </c>
       <c r="BB50" s="16">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BC50" s="16">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BD50" s="16">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE50" s="16">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF50" s="16">
         <f t="shared" si="23"/>
@@ -12600,10 +12494,10 @@
     </row>
     <row r="51" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C51" s="39" t="s">
         <v>77</v>
@@ -12614,7 +12508,7 @@
         <v>4</v>
       </c>
       <c r="G51" s="74" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H51" s="75">
         <v>44529</v>
@@ -12811,8 +12705,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
+    <row r="52" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="65" t="s">
+        <v>146</v>
+      </c>
       <c r="B52" s="26" t="s">
         <v>19</v>
       </c>
@@ -12821,229 +12717,243 @@
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
-      <c r="F52" s="14">
+      <c r="F52" s="66">
         <v>4</v>
       </c>
-      <c r="G52" s="61"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="61"/>
-      <c r="J52" s="67">
+      <c r="G52" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="H52" s="75">
+        <v>44529</v>
+      </c>
+      <c r="I52" s="74">
+        <v>4</v>
+      </c>
+      <c r="J52" s="75">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="K52" s="61"/>
-      <c r="L52" s="61" t="e">
+        <v>44533</v>
+      </c>
+      <c r="K52" s="74"/>
+      <c r="L52" s="74" t="e">
         <f>LOOKUP(K52,TaskGrading!$A$4:$A$7,TaskGrading!$C$4:$C$7)</f>
         <v>#N/A</v>
       </c>
-      <c r="M52" s="61"/>
-      <c r="N52" s="61"/>
-      <c r="O52" s="68"/>
-      <c r="P52" s="67">
+      <c r="M52" s="74"/>
+      <c r="N52" s="74"/>
+      <c r="O52" s="76"/>
+      <c r="P52" s="75">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q52" s="61"/>
-      <c r="R52" s="61"/>
+      <c r="Q52" s="74"/>
+      <c r="R52" s="74" t="s">
+        <v>56</v>
+      </c>
       <c r="S52" s="16">
-        <f t="shared" ref="S52:AB61" si="27">IF(AND(S$6&gt;=$N52,S$6&lt;$N52+$O52), 1, IF(AND(S$6&gt;=$H52,S$6&lt;$H52+$I52), 2, 0))</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="T52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="U52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="V52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="W52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB52" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AC52" s="16">
-        <f t="shared" ref="AC52:AL61" si="28">IF(AND(AC$6&gt;=$N52,AC$6&lt;$N52+$O52), 1, IF(AND(AC$6&gt;=$H52,AC$6&lt;$H52+$I52), 2, 0))</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AE52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AF52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AG52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AH52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AI52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AJ52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AK52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AL52" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AM52" s="16">
-        <f t="shared" ref="AM52:AV61" si="29">IF(AND(AM$6&gt;=$N52,AM$6&lt;$N52+$O52), 1, IF(AND(AM$6&gt;=$H52,AM$6&lt;$H52+$I52), 2, 0))</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AN52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AO52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AP52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AQ52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AS52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AT52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AU52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AV52" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AW52" s="16">
-        <f t="shared" ref="AW52:BF61" si="30">IF(AND(AW$6&gt;=$N52,AW$6&lt;$N52+$O52), 1, IF(AND(AW$6&gt;=$H52,AW$6&lt;$H52+$I52), 2, 0))</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AX52" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AY52" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AZ52" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="BA52" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="BB52" s="16">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2</v>
       </c>
       <c r="BC52" s="16">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2</v>
       </c>
       <c r="BD52" s="16">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2</v>
       </c>
       <c r="BE52" s="16">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2</v>
       </c>
       <c r="BF52" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="BG52" s="16">
-        <f t="shared" ref="BG52:BH61" si="31">IF(AND(BG$6&gt;=$N52,BG$6&lt;$N52+$O52), 1, IF(AND(BG$6&gt;=$H52,BG$6&lt;$H52+$I52), 2, 0))</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="BH52" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="14"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="39"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>77</v>
+      </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="15">
+      <c r="F53" s="14">
+        <v>4</v>
+      </c>
+      <c r="G53" s="61"/>
+      <c r="H53" s="67"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="67">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14" t="e">
+      <c r="K53" s="61"/>
+      <c r="L53" s="61" t="e">
         <f>LOOKUP(K53,TaskGrading!$A$4:$A$7,TaskGrading!$C$4:$C$7)</f>
         <v>#N/A</v>
       </c>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="15">
+      <c r="M53" s="61"/>
+      <c r="N53" s="61"/>
+      <c r="O53" s="68"/>
+      <c r="P53" s="67">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q53" s="14"/>
-      <c r="R53" s="14"/>
+      <c r="Q53" s="61"/>
+      <c r="R53" s="61"/>
       <c r="S53" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="S53:AB62" si="27">IF(AND(S$6&gt;=$N53,S$6&lt;$N53+$O53), 1, IF(AND(S$6&gt;=$H53,S$6&lt;$H53+$I53), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T53" s="16">
@@ -13083,7 +12993,7 @@
         <v>0</v>
       </c>
       <c r="AC53" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="AC53:AL62" si="28">IF(AND(AC$6&gt;=$N53,AC$6&lt;$N53+$O53), 1, IF(AND(AC$6&gt;=$H53,AC$6&lt;$H53+$I53), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD53" s="16">
@@ -13123,7 +13033,7 @@
         <v>0</v>
       </c>
       <c r="AM53" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="AM53:AV62" si="29">IF(AND(AM$6&gt;=$N53,AM$6&lt;$N53+$O53), 1, IF(AND(AM$6&gt;=$H53,AM$6&lt;$H53+$I53), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN53" s="16">
@@ -13163,7 +13073,7 @@
         <v>0</v>
       </c>
       <c r="AW53" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="AW53:BF62" si="30">IF(AND(AW$6&gt;=$N53,AW$6&lt;$N53+$O53), 1, IF(AND(AW$6&gt;=$H53,AW$6&lt;$H53+$I53), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX53" s="16">
@@ -13203,7 +13113,7 @@
         <v>0</v>
       </c>
       <c r="BG53" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="BG53:BH62" si="31">IF(AND(BG$6&gt;=$N53,BG$6&lt;$N53+$O53), 1, IF(AND(BG$6&gt;=$H53,BG$6&lt;$H53+$I53), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH53" s="16">
@@ -14816,171 +14726,171 @@
       <c r="Q62" s="14"/>
       <c r="R62" s="14"/>
       <c r="S62" s="16">
-        <f t="shared" ref="S62:AB71" si="32">IF(AND(S$6&gt;=$N62,S$6&lt;$N62+$O62), 1, IF(AND(S$6&gt;=$H62,S$6&lt;$H62+$I62), 2, 0))</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="T62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="U62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="V62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="W62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="X62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Y62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Z62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AA62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AB62" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AC62" s="16">
-        <f t="shared" ref="AC62:AL71" si="33">IF(AND(AC$6&gt;=$N62,AC$6&lt;$N62+$O62), 1, IF(AND(AC$6&gt;=$H62,AC$6&lt;$H62+$I62), 2, 0))</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AD62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AE62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AF62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AH62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AI62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AK62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AL62" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AM62" s="16">
-        <f t="shared" ref="AM62:AV71" si="34">IF(AND(AM$6&gt;=$N62,AM$6&lt;$N62+$O62), 1, IF(AND(AM$6&gt;=$H62,AM$6&lt;$H62+$I62), 2, 0))</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AN62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AO62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AP62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AQ62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AR62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AS62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AT62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AU62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AV62" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AW62" s="16">
-        <f t="shared" ref="AW62:BF71" si="35">IF(AND(AW$6&gt;=$N62,AW$6&lt;$N62+$O62), 1, IF(AND(AW$6&gt;=$H62,AW$6&lt;$H62+$I62), 2, 0))</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AX62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AY62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AZ62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BA62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BB62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BC62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BD62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BE62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BF62" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="BG62" s="16">
-        <f t="shared" ref="BG62:BH71" si="36">IF(AND(BG$6&gt;=$N62,BG$6&lt;$N62+$O62), 1, IF(AND(BG$6&gt;=$H62,BG$6&lt;$H62+$I62), 2, 0))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="BH62" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -15013,7 +14923,7 @@
       <c r="Q63" s="14"/>
       <c r="R63" s="14"/>
       <c r="S63" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="S63:AB72" si="32">IF(AND(S$6&gt;=$N63,S$6&lt;$N63+$O63), 1, IF(AND(S$6&gt;=$H63,S$6&lt;$H63+$I63), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T63" s="16">
@@ -15053,7 +14963,7 @@
         <v>0</v>
       </c>
       <c r="AC63" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="AC63:AL72" si="33">IF(AND(AC$6&gt;=$N63,AC$6&lt;$N63+$O63), 1, IF(AND(AC$6&gt;=$H63,AC$6&lt;$H63+$I63), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD63" s="16">
@@ -15093,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="AM63" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="AM63:AV72" si="34">IF(AND(AM$6&gt;=$N63,AM$6&lt;$N63+$O63), 1, IF(AND(AM$6&gt;=$H63,AM$6&lt;$H63+$I63), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN63" s="16">
@@ -15133,7 +15043,7 @@
         <v>0</v>
       </c>
       <c r="AW63" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="AW63:BF72" si="35">IF(AND(AW$6&gt;=$N63,AW$6&lt;$N63+$O63), 1, IF(AND(AW$6&gt;=$H63,AW$6&lt;$H63+$I63), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX63" s="16">
@@ -15173,7 +15083,7 @@
         <v>0</v>
       </c>
       <c r="BG63" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="BG63:BH72" si="36">IF(AND(BG$6&gt;=$N63,BG$6&lt;$N63+$O63), 1, IF(AND(BG$6&gt;=$H63,BG$6&lt;$H63+$I63), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH63" s="16">
@@ -16786,171 +16696,171 @@
       <c r="Q72" s="14"/>
       <c r="R72" s="14"/>
       <c r="S72" s="16">
-        <f t="shared" ref="S72:AB81" si="37">IF(AND(S$6&gt;=$N72,S$6&lt;$N72+$O72), 1, IF(AND(S$6&gt;=$H72,S$6&lt;$H72+$I72), 2, 0))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="W72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="X72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Y72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Z72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AA72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB72" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AC72" s="16">
-        <f t="shared" ref="AC72:AL81" si="38">IF(AND(AC$6&gt;=$N72,AC$6&lt;$N72+$O72), 1, IF(AND(AC$6&gt;=$H72,AC$6&lt;$H72+$I72), 2, 0))</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AD72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AE72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AF72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AG72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AH72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AI72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AJ72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AK72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AL72" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AM72" s="16">
-        <f t="shared" ref="AM72:AV81" si="39">IF(AND(AM$6&gt;=$N72,AM$6&lt;$N72+$O72), 1, IF(AND(AM$6&gt;=$H72,AM$6&lt;$H72+$I72), 2, 0))</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AN72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AO72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AP72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AQ72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AR72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AS72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AT72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AU72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AV72" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AW72" s="16">
-        <f t="shared" ref="AW72:BF81" si="40">IF(AND(AW$6&gt;=$N72,AW$6&lt;$N72+$O72), 1, IF(AND(AW$6&gt;=$H72,AW$6&lt;$H72+$I72), 2, 0))</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="AX72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="AY72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="AZ72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BA72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BB72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BC72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BD72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BE72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BF72" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="BG72" s="16">
-        <f t="shared" ref="BG72:BH81" si="41">IF(AND(BG$6&gt;=$N72,BG$6&lt;$N72+$O72), 1, IF(AND(BG$6&gt;=$H72,BG$6&lt;$H72+$I72), 2, 0))</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="BH72" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -16983,7 +16893,7 @@
       <c r="Q73" s="14"/>
       <c r="R73" s="14"/>
       <c r="S73" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="S73:AB82" si="37">IF(AND(S$6&gt;=$N73,S$6&lt;$N73+$O73), 1, IF(AND(S$6&gt;=$H73,S$6&lt;$H73+$I73), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T73" s="16">
@@ -17023,7 +16933,7 @@
         <v>0</v>
       </c>
       <c r="AC73" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="AC73:AL82" si="38">IF(AND(AC$6&gt;=$N73,AC$6&lt;$N73+$O73), 1, IF(AND(AC$6&gt;=$H73,AC$6&lt;$H73+$I73), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD73" s="16">
@@ -17063,7 +16973,7 @@
         <v>0</v>
       </c>
       <c r="AM73" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="AM73:AV82" si="39">IF(AND(AM$6&gt;=$N73,AM$6&lt;$N73+$O73), 1, IF(AND(AM$6&gt;=$H73,AM$6&lt;$H73+$I73), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN73" s="16">
@@ -17103,7 +17013,7 @@
         <v>0</v>
       </c>
       <c r="AW73" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="AW73:BF82" si="40">IF(AND(AW$6&gt;=$N73,AW$6&lt;$N73+$O73), 1, IF(AND(AW$6&gt;=$H73,AW$6&lt;$H73+$I73), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX73" s="16">
@@ -17143,7 +17053,7 @@
         <v>0</v>
       </c>
       <c r="BG73" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="BG73:BH82" si="41">IF(AND(BG$6&gt;=$N73,BG$6&lt;$N73+$O73), 1, IF(AND(BG$6&gt;=$H73,BG$6&lt;$H73+$I73), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH73" s="16">
@@ -18756,171 +18666,171 @@
       <c r="Q82" s="14"/>
       <c r="R82" s="14"/>
       <c r="S82" s="16">
-        <f t="shared" ref="S82:AB91" si="42">IF(AND(S$6&gt;=$N82,S$6&lt;$N82+$O82), 1, IF(AND(S$6&gt;=$H82,S$6&lt;$H82+$I82), 2, 0))</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="T82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="U82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="W82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="X82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Y82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Z82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AA82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AB82" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AC82" s="16">
-        <f t="shared" ref="AC82:AL91" si="43">IF(AND(AC$6&gt;=$N82,AC$6&lt;$N82+$O82), 1, IF(AND(AC$6&gt;=$H82,AC$6&lt;$H82+$I82), 2, 0))</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AD82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AE82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AF82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AG82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AH82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AI82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AJ82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AK82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AL82" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AM82" s="16">
-        <f t="shared" ref="AM82:AV91" si="44">IF(AND(AM$6&gt;=$N82,AM$6&lt;$N82+$O82), 1, IF(AND(AM$6&gt;=$H82,AM$6&lt;$H82+$I82), 2, 0))</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AN82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AO82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AP82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AQ82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AR82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AS82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AT82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AU82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AV82" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AW82" s="16">
-        <f t="shared" ref="AW82:BF91" si="45">IF(AND(AW$6&gt;=$N82,AW$6&lt;$N82+$O82), 1, IF(AND(AW$6&gt;=$H82,AW$6&lt;$H82+$I82), 2, 0))</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AX82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AY82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AZ82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BA82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BB82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BC82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BD82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BE82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BF82" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="BG82" s="16">
-        <f t="shared" ref="BG82:BH91" si="46">IF(AND(BG$6&gt;=$N82,BG$6&lt;$N82+$O82), 1, IF(AND(BG$6&gt;=$H82,BG$6&lt;$H82+$I82), 2, 0))</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="BH82" s="16">
-        <f t="shared" si="46"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
     </row>
@@ -18953,7 +18863,7 @@
       <c r="Q83" s="14"/>
       <c r="R83" s="14"/>
       <c r="S83" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="S83:AB92" si="42">IF(AND(S$6&gt;=$N83,S$6&lt;$N83+$O83), 1, IF(AND(S$6&gt;=$H83,S$6&lt;$H83+$I83), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T83" s="16">
@@ -18993,7 +18903,7 @@
         <v>0</v>
       </c>
       <c r="AC83" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="AC83:AL92" si="43">IF(AND(AC$6&gt;=$N83,AC$6&lt;$N83+$O83), 1, IF(AND(AC$6&gt;=$H83,AC$6&lt;$H83+$I83), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD83" s="16">
@@ -19033,7 +18943,7 @@
         <v>0</v>
       </c>
       <c r="AM83" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="AM83:AV92" si="44">IF(AND(AM$6&gt;=$N83,AM$6&lt;$N83+$O83), 1, IF(AND(AM$6&gt;=$H83,AM$6&lt;$H83+$I83), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN83" s="16">
@@ -19073,7 +18983,7 @@
         <v>0</v>
       </c>
       <c r="AW83" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="AW83:BF92" si="45">IF(AND(AW$6&gt;=$N83,AW$6&lt;$N83+$O83), 1, IF(AND(AW$6&gt;=$H83,AW$6&lt;$H83+$I83), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX83" s="16">
@@ -19113,7 +19023,7 @@
         <v>0</v>
       </c>
       <c r="BG83" s="16">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="BG83:BH92" si="46">IF(AND(BG$6&gt;=$N83,BG$6&lt;$N83+$O83), 1, IF(AND(BG$6&gt;=$H83,BG$6&lt;$H83+$I83), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH83" s="16">
@@ -19920,7 +19830,7 @@
       <c r="H88" s="15"/>
       <c r="I88" s="14"/>
       <c r="J88" s="15">
-        <f t="shared" ref="J88:J115" si="47">H88 +I88</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K88" s="14"/>
@@ -19932,7 +19842,7 @@
       <c r="N88" s="14"/>
       <c r="O88" s="17"/>
       <c r="P88" s="15">
-        <f t="shared" ref="P88:P115" si="48">N88+O88</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q88" s="14"/>
@@ -20117,7 +20027,7 @@
       <c r="H89" s="15"/>
       <c r="I89" s="14"/>
       <c r="J89" s="15">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="J89:J116" si="47">H89 +I89</f>
         <v>0</v>
       </c>
       <c r="K89" s="14"/>
@@ -20129,7 +20039,7 @@
       <c r="N89" s="14"/>
       <c r="O89" s="17"/>
       <c r="P89" s="15">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="P89:P116" si="48">N89+O89</f>
         <v>0</v>
       </c>
       <c r="Q89" s="14"/>
@@ -20726,171 +20636,171 @@
       <c r="Q92" s="14"/>
       <c r="R92" s="14"/>
       <c r="S92" s="16">
-        <f t="shared" ref="S92:AB101" si="49">IF(AND(S$6&gt;=$N92,S$6&lt;$N92+$O92), 1, IF(AND(S$6&gt;=$H92,S$6&lt;$H92+$I92), 2, 0))</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="T92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="U92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="V92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="W92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="X92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Y92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Z92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AA92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AB92" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AC92" s="16">
-        <f t="shared" ref="AC92:AL101" si="50">IF(AND(AC$6&gt;=$N92,AC$6&lt;$N92+$O92), 1, IF(AND(AC$6&gt;=$H92,AC$6&lt;$H92+$I92), 2, 0))</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AD92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AE92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AF92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AG92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AH92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AI92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AJ92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AK92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AL92" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AM92" s="16">
-        <f t="shared" ref="AM92:AV101" si="51">IF(AND(AM$6&gt;=$N92,AM$6&lt;$N92+$O92), 1, IF(AND(AM$6&gt;=$H92,AM$6&lt;$H92+$I92), 2, 0))</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AN92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AO92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AP92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AQ92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AR92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AS92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AT92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AU92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AV92" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AW92" s="16">
-        <f t="shared" ref="AW92:BF101" si="52">IF(AND(AW$6&gt;=$N92,AW$6&lt;$N92+$O92), 1, IF(AND(AW$6&gt;=$H92,AW$6&lt;$H92+$I92), 2, 0))</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AX92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AY92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AZ92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BA92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BB92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BC92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BD92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BE92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BF92" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="BG92" s="16">
-        <f t="shared" ref="BG92:BH101" si="53">IF(AND(BG$6&gt;=$N92,BG$6&lt;$N92+$O92), 1, IF(AND(BG$6&gt;=$H92,BG$6&lt;$H92+$I92), 2, 0))</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="BH92" s="16">
-        <f t="shared" si="53"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
@@ -20923,7 +20833,7 @@
       <c r="Q93" s="14"/>
       <c r="R93" s="14"/>
       <c r="S93" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="S93:AB102" si="49">IF(AND(S$6&gt;=$N93,S$6&lt;$N93+$O93), 1, IF(AND(S$6&gt;=$H93,S$6&lt;$H93+$I93), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T93" s="16">
@@ -20963,7 +20873,7 @@
         <v>0</v>
       </c>
       <c r="AC93" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="AC93:AL102" si="50">IF(AND(AC$6&gt;=$N93,AC$6&lt;$N93+$O93), 1, IF(AND(AC$6&gt;=$H93,AC$6&lt;$H93+$I93), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD93" s="16">
@@ -21003,7 +20913,7 @@
         <v>0</v>
       </c>
       <c r="AM93" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" ref="AM93:AV102" si="51">IF(AND(AM$6&gt;=$N93,AM$6&lt;$N93+$O93), 1, IF(AND(AM$6&gt;=$H93,AM$6&lt;$H93+$I93), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN93" s="16">
@@ -21043,7 +20953,7 @@
         <v>0</v>
       </c>
       <c r="AW93" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="AW93:BF102" si="52">IF(AND(AW$6&gt;=$N93,AW$6&lt;$N93+$O93), 1, IF(AND(AW$6&gt;=$H93,AW$6&lt;$H93+$I93), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX93" s="16">
@@ -21083,7 +20993,7 @@
         <v>0</v>
       </c>
       <c r="BG93" s="16">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="BG93:BH102" si="53">IF(AND(BG$6&gt;=$N93,BG$6&lt;$N93+$O93), 1, IF(AND(BG$6&gt;=$H93,BG$6&lt;$H93+$I93), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH93" s="16">
@@ -22696,171 +22606,171 @@
       <c r="Q102" s="14"/>
       <c r="R102" s="14"/>
       <c r="S102" s="16">
-        <f t="shared" ref="S102:AB115" si="54">IF(AND(S$6&gt;=$N102,S$6&lt;$N102+$O102), 1, IF(AND(S$6&gt;=$H102,S$6&lt;$H102+$I102), 2, 0))</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="T102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="U102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="V102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="W102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="X102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Y102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="AA102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="AB102" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="AC102" s="16">
-        <f t="shared" ref="AC102:AL115" si="55">IF(AND(AC$6&gt;=$N102,AC$6&lt;$N102+$O102), 1, IF(AND(AC$6&gt;=$H102,AC$6&lt;$H102+$I102), 2, 0))</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AD102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AE102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AF102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AG102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AH102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AI102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AJ102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AK102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AL102" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AM102" s="16">
-        <f t="shared" ref="AM102:AV115" si="56">IF(AND(AM$6&gt;=$N102,AM$6&lt;$N102+$O102), 1, IF(AND(AM$6&gt;=$H102,AM$6&lt;$H102+$I102), 2, 0))</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AN102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AO102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AP102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AQ102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AR102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AS102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AT102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AU102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AV102" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AW102" s="16">
-        <f t="shared" ref="AW102:BF115" si="57">IF(AND(AW$6&gt;=$N102,AW$6&lt;$N102+$O102), 1, IF(AND(AW$6&gt;=$H102,AW$6&lt;$H102+$I102), 2, 0))</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="AX102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="AY102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="AZ102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BA102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BB102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BC102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BD102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BE102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BF102" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="BG102" s="16">
-        <f t="shared" ref="BG102:BH115" si="58">IF(AND(BG$6&gt;=$N102,BG$6&lt;$N102+$O102), 1, IF(AND(BG$6&gt;=$H102,BG$6&lt;$H102+$I102), 2, 0))</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="BH102" s="16">
-        <f t="shared" si="58"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
     </row>
@@ -22893,7 +22803,7 @@
       <c r="Q103" s="14"/>
       <c r="R103" s="14"/>
       <c r="S103" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="S103:AB116" si="54">IF(AND(S$6&gt;=$N103,S$6&lt;$N103+$O103), 1, IF(AND(S$6&gt;=$H103,S$6&lt;$H103+$I103), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="T103" s="16">
@@ -22933,7 +22843,7 @@
         <v>0</v>
       </c>
       <c r="AC103" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" ref="AC103:AL116" si="55">IF(AND(AC$6&gt;=$N103,AC$6&lt;$N103+$O103), 1, IF(AND(AC$6&gt;=$H103,AC$6&lt;$H103+$I103), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AD103" s="16">
@@ -22973,7 +22883,7 @@
         <v>0</v>
       </c>
       <c r="AM103" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" ref="AM103:AV116" si="56">IF(AND(AM$6&gt;=$N103,AM$6&lt;$N103+$O103), 1, IF(AND(AM$6&gt;=$H103,AM$6&lt;$H103+$I103), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AN103" s="16">
@@ -23013,7 +22923,7 @@
         <v>0</v>
       </c>
       <c r="AW103" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" ref="AW103:BF116" si="57">IF(AND(AW$6&gt;=$N103,AW$6&lt;$N103+$O103), 1, IF(AND(AW$6&gt;=$H103,AW$6&lt;$H103+$I103), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="AX103" s="16">
@@ -23053,7 +22963,7 @@
         <v>0</v>
       </c>
       <c r="BG103" s="16">
-        <f t="shared" si="58"/>
+        <f t="shared" ref="BG103:BH116" si="58">IF(AND(BG$6&gt;=$N103,BG$6&lt;$N103+$O103), 1, IF(AND(BG$6&gt;=$H103,BG$6&lt;$H103+$I103), 2, 0))</f>
         <v>0</v>
       </c>
       <c r="BH103" s="16">
@@ -25242,6 +25152,7 @@
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
+      <c r="K115" s="14"/>
       <c r="L115" s="14" t="e">
         <f>LOOKUP(K115,TaskGrading!$A$4:$A$7,TaskGrading!$C$4:$C$7)</f>
         <v>#N/A</v>
@@ -25420,6 +25331,202 @@
         <v>0</v>
       </c>
       <c r="BH115" s="16">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:60" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="14"/>
+      <c r="B116" s="26"/>
+      <c r="C116" s="39"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="15"/>
+      <c r="I116" s="14"/>
+      <c r="J116" s="15">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="L116" s="14" t="e">
+        <f>LOOKUP(K116,TaskGrading!$A$4:$A$7,TaskGrading!$C$4:$C$7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M116" s="14"/>
+      <c r="N116" s="14"/>
+      <c r="O116" s="17"/>
+      <c r="P116" s="15">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="Q116" s="14"/>
+      <c r="R116" s="14"/>
+      <c r="S116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="T116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="U116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="V116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="W116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="X116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Y116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Z116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AA116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AB116" s="16">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AC116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AD116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AE116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AF116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AG116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AH116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AI116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AJ116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AK116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AL116" s="16">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="AM116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AN116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AO116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AP116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AQ116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AR116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AS116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AT116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AU116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AV116" s="16">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AW116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="AX116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="AY116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="AZ116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BA116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BB116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BC116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BD116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BE116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BF116" s="16">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="BG116" s="16">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="BH116" s="16">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
@@ -25451,367 +25558,372 @@
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="D6:D7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A11:A14 L10:P11 L8:BH9 R10:BH11 A18 A23:A24 A35:A36 D27:F27 A43 D38:F43 H38:J43 L45:BH48 A52:A115 D45:F46 D52:J115 D48:F48 H45:J46 D47:J47 H48:J48 L50:BH115 D50:F51 H50:J51 D8:J26 H27:J28 D34:J37 E28:F28 L12:BH28 H31:J33 D31:F33 L31:BH43 E30">
-    <cfRule type="expression" dxfId="180" priority="75" stopIfTrue="1">
+  <conditionalFormatting sqref="A11:A14 L10:P11 L8:BH9 R10:BH11 A18 A23:A24 A36:A37 D27:F27 A44 D39:F44 H39:J44 L46:BH49 A53:A116 D46:F47 D53:J116 D49:F49 H46:J47 D48:J48 H49:J49 L51:BH116 D51:F52 H51:J52 D8:J26 H27:J28 D34:J38 E28:F28 L12:BH28 H31:J33 D31:F33 L31:BH44 E30">
+    <cfRule type="expression" dxfId="188" priority="75" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A8)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:BH43 S45:BH48 S50:BH115">
-    <cfRule type="expression" dxfId="179" priority="73">
+  <conditionalFormatting sqref="S8:BH44 S46:BH49 S51:BH116">
+    <cfRule type="expression" dxfId="187" priority="73">
       <formula>S$6=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="74">
+    <cfRule type="expression" dxfId="186" priority="74">
       <formula>OR(WEEKDAY(S$6,2)=6,WEEKDAY(S$6,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:BH26 S29:BH29 S32:BH43 S45:BH48 S50:BH115">
-    <cfRule type="expression" dxfId="177" priority="78" stopIfTrue="1">
+  <conditionalFormatting sqref="S8:BH26 S29:BH29 S32:BH44 S46:BH49 S51:BH116">
+    <cfRule type="expression" dxfId="185" priority="78" stopIfTrue="1">
       <formula>SEARCH("SPACER",$G8)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15:S16">
-    <cfRule type="expression" dxfId="176" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="88" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A15)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:BH43 S45:BH48 S50:BH115">
-    <cfRule type="cellIs" dxfId="175" priority="87" operator="equal">
+  <conditionalFormatting sqref="S8:BH44 S46:BH49 S51:BH116">
+    <cfRule type="cellIs" dxfId="183" priority="87" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:BH43 S45:BH48 S50:BH115">
-    <cfRule type="cellIs" dxfId="174" priority="86" operator="equal">
+  <conditionalFormatting sqref="S8:BH44 S46:BH49 S51:BH116">
+    <cfRule type="cellIs" dxfId="182" priority="86" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8:BH43 S45:BH48 S50:BH115">
-    <cfRule type="cellIs" dxfId="173" priority="80" operator="equal">
+  <conditionalFormatting sqref="S8:BH44 S46:BH49 S51:BH116">
+    <cfRule type="cellIs" dxfId="181" priority="80" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11 B45:C48 B50:C115 B13:C17 B24:C43 B20:C21 B18:B23">
-    <cfRule type="containsText" dxfId="172" priority="63" operator="containsText" text="Bug Fix">
+  <conditionalFormatting sqref="B11:C11 B46:C49 B51:C116 B13:C17 B24:C44 B20:C21 B18:B23">
+    <cfRule type="containsText" dxfId="180" priority="63" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="64" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="179" priority="64" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="65" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="178" priority="65" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="66" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="177" priority="66" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="67" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="176" priority="67" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q10 K23 K26 K35:K36 K38:K39 K41:K43 K45:K48 K50:K114 K13:K14 K17 L29:BH29 F29:J29 D29">
-    <cfRule type="expression" dxfId="167" priority="90" stopIfTrue="1">
+  <conditionalFormatting sqref="Q10 K23 K26 K36:K37 K39:K40 K42:K44 K46:K49 K51:K115 K13:K14 K17 L29:BH29 F29:J29 D29">
+    <cfRule type="expression" dxfId="175" priority="90" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A11)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10">
-    <cfRule type="containsText" dxfId="166" priority="58" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="174" priority="58" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="59" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="173" priority="59" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="60" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="172" priority="60" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="61" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="171" priority="61" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="62" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="170" priority="62" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C10">
-    <cfRule type="containsText" dxfId="161" priority="53" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="169" priority="53" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="54" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="168" priority="54" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="55" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="167" priority="55" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="56" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="166" priority="56" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="57" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="165" priority="57" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10 K8 K21 K33:K34">
-    <cfRule type="expression" dxfId="156" priority="91" stopIfTrue="1">
+  <conditionalFormatting sqref="K10 K8 K21">
+    <cfRule type="expression" dxfId="164" priority="91" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A11)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K12 K24:K25 K15:K16">
-    <cfRule type="expression" dxfId="155" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="93" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A13)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9 K20 K22 K32">
-    <cfRule type="expression" dxfId="154" priority="96" stopIfTrue="1">
+  <conditionalFormatting sqref="K9 K20 K22 K33:K35">
+    <cfRule type="expression" dxfId="162" priority="96" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A13)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="expression" dxfId="153" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="52" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A12)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18:K19 K31">
-    <cfRule type="expression" dxfId="152" priority="99" stopIfTrue="1">
+  <conditionalFormatting sqref="K18:K19 K32">
+    <cfRule type="expression" dxfId="160" priority="99" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A23)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="expression" dxfId="151" priority="100" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A36)=1</formula>
+    <cfRule type="expression" dxfId="159" priority="100" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A37)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28 G42 L30:BH30 G32 F30:J30 D30">
-    <cfRule type="expression" dxfId="150" priority="102" stopIfTrue="1">
+  <conditionalFormatting sqref="G28 G43 L30:BH30 G32 F30:J30 D30">
+    <cfRule type="expression" dxfId="158" priority="102" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A27)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S30:BH30 S27:BH27">
-    <cfRule type="expression" dxfId="149" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="104" stopIfTrue="1">
       <formula>SEARCH("SPACER",$G28)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31:BH31 S28:BH28">
-    <cfRule type="expression" dxfId="148" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="105" stopIfTrue="1">
       <formula>SEARCH("SPACER",#REF!)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:K28">
-    <cfRule type="expression" dxfId="147" priority="106" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A35)=1</formula>
+    <cfRule type="expression" dxfId="155" priority="106" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A36)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="expression" dxfId="146" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="50" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A26)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="expression" dxfId="145" priority="110" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A36)=1</formula>
+    <cfRule type="expression" dxfId="153" priority="110" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A37)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40 G43">
-    <cfRule type="expression" dxfId="144" priority="48" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A40)=1</formula>
+  <conditionalFormatting sqref="G41 G44">
+    <cfRule type="expression" dxfId="152" priority="48" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A41)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
-    <cfRule type="expression" dxfId="143" priority="49" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A38)=1</formula>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="expression" dxfId="151" priority="49" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A39)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38 G41">
-    <cfRule type="expression" dxfId="142" priority="46" stopIfTrue="1">
+  <conditionalFormatting sqref="G39 G42">
+    <cfRule type="expression" dxfId="150" priority="46" stopIfTrue="1">
       <formula>SEARCH("SPACER",#REF!)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K37 K40">
-    <cfRule type="expression" dxfId="141" priority="141" stopIfTrue="1">
+  <conditionalFormatting sqref="K38 K41">
+    <cfRule type="expression" dxfId="149" priority="141" stopIfTrue="1">
       <formula>SEARCH("SPACER",#REF!)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44 D44:J44 L44:BH44">
-    <cfRule type="expression" dxfId="140" priority="40" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A44)=1</formula>
+  <conditionalFormatting sqref="A45 D45:J45 L45:BH45">
+    <cfRule type="expression" dxfId="148" priority="40" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A45)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S44:BH44">
-    <cfRule type="expression" dxfId="139" priority="38">
+  <conditionalFormatting sqref="S45:BH45">
+    <cfRule type="expression" dxfId="147" priority="38">
       <formula>S$6=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="39">
+    <cfRule type="expression" dxfId="146" priority="39">
       <formula>OR(WEEKDAY(S$6,2)=6,WEEKDAY(S$6,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S44:BH44">
-    <cfRule type="expression" dxfId="137" priority="41" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$G44)=1</formula>
+  <conditionalFormatting sqref="S45:BH45">
+    <cfRule type="expression" dxfId="145" priority="41" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$G45)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S44:BH44">
-    <cfRule type="cellIs" dxfId="136" priority="44" operator="equal">
+  <conditionalFormatting sqref="S45:BH45">
+    <cfRule type="cellIs" dxfId="144" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S44:BH44">
-    <cfRule type="cellIs" dxfId="135" priority="43" operator="equal">
+  <conditionalFormatting sqref="S45:BH45">
+    <cfRule type="cellIs" dxfId="143" priority="43" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S44:BH44">
-    <cfRule type="cellIs" dxfId="134" priority="42" operator="equal">
+  <conditionalFormatting sqref="S45:BH45">
+    <cfRule type="cellIs" dxfId="142" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:C44">
-    <cfRule type="containsText" dxfId="133" priority="33" operator="containsText" text="Bug Fix">
-      <formula>NOT(ISERROR(SEARCH("Bug Fix",B44)))</formula>
+  <conditionalFormatting sqref="B45:C45">
+    <cfRule type="containsText" dxfId="141" priority="33" operator="containsText" text="Bug Fix">
+      <formula>NOT(ISERROR(SEARCH("Bug Fix",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="34" operator="containsText" text="Code">
-      <formula>NOT(ISERROR(SEARCH("Code",B44)))</formula>
+    <cfRule type="containsText" dxfId="140" priority="34" operator="containsText" text="Code">
+      <formula>NOT(ISERROR(SEARCH("Code",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="35" operator="containsText" text="Audio">
-      <formula>NOT(ISERROR(SEARCH("Audio",B44)))</formula>
+    <cfRule type="containsText" dxfId="139" priority="35" operator="containsText" text="Audio">
+      <formula>NOT(ISERROR(SEARCH("Audio",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="36" operator="containsText" text="Level">
-      <formula>NOT(ISERROR(SEARCH("Level",B44)))</formula>
+    <cfRule type="containsText" dxfId="138" priority="36" operator="containsText" text="Level">
+      <formula>NOT(ISERROR(SEARCH("Level",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="37" operator="containsText" text="Art">
-      <formula>NOT(ISERROR(SEARCH("Art",B44)))</formula>
+    <cfRule type="containsText" dxfId="137" priority="37" operator="containsText" text="Art">
+      <formula>NOT(ISERROR(SEARCH("Art",B45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="128" priority="45" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A45)=1</formula>
+  <conditionalFormatting sqref="K45">
+    <cfRule type="expression" dxfId="136" priority="45" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A46)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="127" priority="32" stopIfTrue="1">
+  <conditionalFormatting sqref="G46">
+    <cfRule type="expression" dxfId="135" priority="32" stopIfTrue="1">
       <formula>SEARCH("SPACER",#REF!)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="expression" dxfId="126" priority="31" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A46)=1</formula>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="expression" dxfId="134" priority="31" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A47)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
-    <cfRule type="expression" dxfId="125" priority="30" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A48)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49 D49:J49 L49:BH49">
-    <cfRule type="expression" dxfId="124" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="G49">
+    <cfRule type="expression" dxfId="133" priority="30" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A49)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S49:BH49">
-    <cfRule type="expression" dxfId="123" priority="22">
+  <conditionalFormatting sqref="A50 D50:J50 L50:BH50">
+    <cfRule type="expression" dxfId="132" priority="24" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A50)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S50:BH50">
+    <cfRule type="expression" dxfId="131" priority="22">
       <formula>S$6=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="23">
+    <cfRule type="expression" dxfId="130" priority="23">
       <formula>OR(WEEKDAY(S$6,2)=6,WEEKDAY(S$6,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S49:BH49">
-    <cfRule type="expression" dxfId="121" priority="25" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$G49)=1</formula>
+  <conditionalFormatting sqref="S50:BH50">
+    <cfRule type="expression" dxfId="129" priority="25" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$G50)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S49:BH49">
-    <cfRule type="cellIs" dxfId="120" priority="28" operator="equal">
+  <conditionalFormatting sqref="S50:BH50">
+    <cfRule type="cellIs" dxfId="128" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S49:BH49">
-    <cfRule type="cellIs" dxfId="119" priority="27" operator="equal">
+  <conditionalFormatting sqref="S50:BH50">
+    <cfRule type="cellIs" dxfId="127" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S49:BH49">
-    <cfRule type="cellIs" dxfId="118" priority="26" operator="equal">
+  <conditionalFormatting sqref="S50:BH50">
+    <cfRule type="cellIs" dxfId="126" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49:C49">
-    <cfRule type="containsText" dxfId="117" priority="17" operator="containsText" text="Bug Fix">
-      <formula>NOT(ISERROR(SEARCH("Bug Fix",B49)))</formula>
+  <conditionalFormatting sqref="B50:C50">
+    <cfRule type="containsText" dxfId="125" priority="17" operator="containsText" text="Bug Fix">
+      <formula>NOT(ISERROR(SEARCH("Bug Fix",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="18" operator="containsText" text="Code">
-      <formula>NOT(ISERROR(SEARCH("Code",B49)))</formula>
+    <cfRule type="containsText" dxfId="124" priority="18" operator="containsText" text="Code">
+      <formula>NOT(ISERROR(SEARCH("Code",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="19" operator="containsText" text="Audio">
-      <formula>NOT(ISERROR(SEARCH("Audio",B49)))</formula>
+    <cfRule type="containsText" dxfId="123" priority="19" operator="containsText" text="Audio">
+      <formula>NOT(ISERROR(SEARCH("Audio",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="20" operator="containsText" text="Level">
-      <formula>NOT(ISERROR(SEARCH("Level",B49)))</formula>
+    <cfRule type="containsText" dxfId="122" priority="20" operator="containsText" text="Level">
+      <formula>NOT(ISERROR(SEARCH("Level",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="21" operator="containsText" text="Art">
-      <formula>NOT(ISERROR(SEARCH("Art",B49)))</formula>
+    <cfRule type="containsText" dxfId="121" priority="21" operator="containsText" text="Art">
+      <formula>NOT(ISERROR(SEARCH("Art",B50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K49">
-    <cfRule type="expression" dxfId="112" priority="29" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A50)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="expression" dxfId="111" priority="16" stopIfTrue="1">
-      <formula>SEARCH("SPACER",$A50)=1</formula>
+  <conditionalFormatting sqref="K50">
+    <cfRule type="expression" dxfId="120" priority="29" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A51)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="110" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="16" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A51)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G52">
+    <cfRule type="expression" dxfId="118" priority="15" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A52)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="109" priority="10" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="117" priority="10" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="11" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="116" priority="11" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="12" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="115" priority="12" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="13" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="114" priority="13" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="14" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="113" priority="14" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="104" priority="5" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="112" priority="5" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="6" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="111" priority="6" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="7" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="110" priority="7" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="8" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="109" priority="8" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="9" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="108" priority="9" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="expression" dxfId="99" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="4" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A32)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="98" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="3" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A28)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="expression" dxfId="97" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="151" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A29)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="96" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="153" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A29)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="expression" dxfId="103" priority="156" stopIfTrue="1">
+      <formula>SEARCH("SPACER",$A37)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25853,31 +25965,31 @@
           <x14:formula1>
             <xm:f>TaskTypes!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B8:B110</xm:sqref>
+          <xm:sqref>B8:B111</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>TaskGrading!$A$4:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>K8:K114</xm:sqref>
+          <xm:sqref>K8:K115</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>TaskStatus!$A$6:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>R8:R115</xm:sqref>
+          <xm:sqref>R8:R116</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8AF4FB63-5986-4C21-AFB9-6703D4D46921}">
           <x14:formula1>
             <xm:f>Priorities!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C24:C115 C8:C17 C20:C21</xm:sqref>
+          <xm:sqref>C24:C116 C8:C17 C20:C21</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Main!$A$9:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>G8:G115</xm:sqref>
+          <xm:sqref>G8:G116</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -26552,309 +26664,309 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="containsText" dxfId="95" priority="85" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="102" priority="85" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="86" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="101" priority="86" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="87" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="100" priority="87" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="88" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="89" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="98" priority="89" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7 BG7:BH7 C7 E7 G7 I7 K7 M7 O7 Q7 S7 U7 W7 Y7 AA7 AC7 AE7 AG7 AI7 AK7 AM7 AO7 AQ7 AS7 AU7 AW7 AY7 BA7 BC7 BE7">
-    <cfRule type="expression" dxfId="90" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="79" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A7)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG7:BH7">
-    <cfRule type="expression" dxfId="89" priority="77">
+    <cfRule type="expression" dxfId="96" priority="77">
       <formula>BG$6=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="78">
+    <cfRule type="expression" dxfId="95" priority="78">
       <formula>OR(WEEKDAY(BG$6,2)=6,WEEKDAY(BG$6,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG7:BH7">
-    <cfRule type="expression" dxfId="87" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="80" stopIfTrue="1">
       <formula>SEARCH("SPACER",$G7)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG7:BH7">
-    <cfRule type="cellIs" dxfId="86" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="83" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG7:BH7">
-    <cfRule type="cellIs" dxfId="85" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="82" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG7:BH7">
-    <cfRule type="cellIs" dxfId="84" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="81" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7 D7 F7 H7 J7 L7 N7 P7 R7 T7 V7 X7 Z7 AB7 AD7 AF7 AH7 AJ7 AL7 AN7 AP7 AR7 AT7 AV7 AX7 AZ7 BB7 BD7 BF7">
-    <cfRule type="expression" dxfId="83" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="71" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A7)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="expression" dxfId="82" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="70" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A11)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="containsText" dxfId="81" priority="65" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="88" priority="65" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="66" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="87" priority="66" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="67" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="86" priority="67" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="68" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="85" priority="68" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="69" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="84" priority="69" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="76" priority="60" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="83" priority="60" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="61" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="82" priority="61" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="62" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="63" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="80" priority="63" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="79" priority="64" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="containsText" dxfId="71" priority="55" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="78" priority="55" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="56" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="77" priority="56" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="57" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="58" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="75" priority="58" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="59" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="74" priority="59" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="66" priority="50" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="73" priority="50" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="51" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="72" priority="51" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="52" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="53" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="70" priority="53" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="54" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="69" priority="54" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="containsText" dxfId="61" priority="45" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="68" priority="45" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="46" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="67" priority="46" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="47" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="66" priority="47" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="48" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="65" priority="48" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="49" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="64" priority="49" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="containsText" dxfId="56" priority="40" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="63" priority="40" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="41" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="62" priority="41" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="42" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="61" priority="42" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="43" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="60" priority="43" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="44" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="59" priority="44" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14 BG14:BH14 C14 E14 G14 I14 K14 M14 O14 Q14 S14 U14 W14 Y14 AA14 AC14 AE14 AG14 AI14 AK14 AM14 AO14 AQ14 AS14 AU14 AW14 AY14 BA14 BC14 BE14">
-    <cfRule type="expression" dxfId="51" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="35" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A14)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG14:BH14">
-    <cfRule type="expression" dxfId="50" priority="33">
+    <cfRule type="expression" dxfId="57" priority="33">
       <formula>BG$6=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="34">
+    <cfRule type="expression" dxfId="56" priority="34">
       <formula>OR(WEEKDAY(BG$6,2)=6,WEEKDAY(BG$6,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG14:BH14">
-    <cfRule type="expression" dxfId="48" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
       <formula>SEARCH("SPACER",$G14)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG14:BH14">
-    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG14:BH14">
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="38" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG14:BH14">
-    <cfRule type="cellIs" dxfId="45" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14 D14 F14 H14 J14 L14 N14 P14 R14 T14 V14 X14 Z14 AB14 AD14 AF14 AH14 AJ14 AL14 AN14 AP14 AR14 AT14 AV14 AX14 AZ14 BB14 BD14 BF14">
-    <cfRule type="expression" dxfId="44" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="32" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A14)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17 B22">
-    <cfRule type="expression" dxfId="43" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="31" stopIfTrue="1">
       <formula>SEARCH("SPACER",$A17)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="containsText" dxfId="42" priority="26" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="49" priority="26" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="27" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="48" priority="27" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="28" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="29" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="46" priority="29" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="30" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="45" priority="30" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="37" priority="21" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="44" priority="21" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="22" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="43" priority="22" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="23" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="42" priority="23" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="24" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="41" priority="24" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="25" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="40" priority="25" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="containsText" dxfId="32" priority="16" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="39" priority="16" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="17" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="36" priority="19" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="35" priority="20" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="12" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Bug Fix">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="Bug Fix">
       <formula>NOT(ISERROR(SEARCH("Bug Fix",A22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Code">
+    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="Code">
       <formula>NOT(ISERROR(SEARCH("Code",A22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Audio">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Audio">
       <formula>NOT(ISERROR(SEARCH("Audio",A22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Level">
+    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="Level">
       <formula>NOT(ISERROR(SEARCH("Level",A22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Art">
+    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="Art">
       <formula>NOT(ISERROR(SEARCH("Art",A22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26957,29 +27069,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A7">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A7">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",A5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",A5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",A5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27092,24 +27204,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="GREEN">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="GREEN">
       <formula>NOT(ISERROR(SEARCH("GREEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="YELLOW">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="YELLOW">
       <formula>NOT(ISERROR(SEARCH("YELLOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="RED">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="RED">
       <formula>NOT(ISERROR(SEARCH("RED",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="GREEN">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="GREEN">
       <formula>NOT(ISERROR(SEARCH("GREEN",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YELLOW">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="YELLOW">
       <formula>NOT(ISERROR(SEARCH("YELLOW",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="RED">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="RED">
       <formula>NOT(ISERROR(SEARCH("RED",A3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update task description of production plan
</commit_message>
<xml_diff>
--- a/Skeleton_Party_production_plan.xlsx
+++ b/Skeleton_Party_production_plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raidzer\Documents\GitHub\Skeleton-Party\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\Documents\GitHub\Skeleton-Party\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348F67ED-6817-441B-A2A1-0B6E05817569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336DF426-3915-4454-9402-1B1B4AA03D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="207">
   <si>
     <t>TASK</t>
   </si>
@@ -981,6 +981,15 @@
   <si>
     <t>Updated Paue UI</t>
   </si>
+  <si>
+    <t>Transition between game states of main menu, pause, playing, exit, etc</t>
+  </si>
+  <si>
+    <t>Enemy drops include healing items, temporary buffs,etc</t>
+  </si>
+  <si>
+    <t>Updated the main menu design</t>
+  </si>
 </sst>
 </file>
 
@@ -1737,7 +1746,28 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1746,31 +1776,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4503,21 +4512,21 @@
   <dimension ref="A1:BZ117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="18" ySplit="7" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="18" ySplit="7" topLeftCell="AE32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="O43" sqref="O43"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="22" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="14.33203125" style="22" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="245.5546875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="20.88671875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="22.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" style="22" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="14.33203125" style="22" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="245.5546875" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="20.88671875" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" style="54" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.44140625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -4593,66 +4602,66 @@
       <c r="Q5" s="8">
         <v>357</v>
       </c>
-      <c r="S5" s="87">
+      <c r="S5" s="91">
         <f>$G$2-350+$Q$5</f>
         <v>44494</v>
       </c>
-      <c r="T5" s="87"/>
-      <c r="U5" s="87"/>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87"/>
-      <c r="Z5" s="87">
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
+      <c r="W5" s="91"/>
+      <c r="X5" s="91"/>
+      <c r="Y5" s="91"/>
+      <c r="Z5" s="91">
         <f>S5+7</f>
         <v>44501</v>
       </c>
-      <c r="AA5" s="87"/>
-      <c r="AB5" s="87"/>
-      <c r="AC5" s="87"/>
-      <c r="AD5" s="87"/>
-      <c r="AE5" s="87"/>
-      <c r="AF5" s="87"/>
-      <c r="AG5" s="87">
+      <c r="AA5" s="91"/>
+      <c r="AB5" s="91"/>
+      <c r="AC5" s="91"/>
+      <c r="AD5" s="91"/>
+      <c r="AE5" s="91"/>
+      <c r="AF5" s="91"/>
+      <c r="AG5" s="91">
         <f>Z5+7</f>
         <v>44508</v>
       </c>
-      <c r="AH5" s="87"/>
-      <c r="AI5" s="87"/>
-      <c r="AJ5" s="87"/>
-      <c r="AK5" s="87"/>
-      <c r="AL5" s="87"/>
-      <c r="AM5" s="87"/>
-      <c r="AN5" s="87">
+      <c r="AH5" s="91"/>
+      <c r="AI5" s="91"/>
+      <c r="AJ5" s="91"/>
+      <c r="AK5" s="91"/>
+      <c r="AL5" s="91"/>
+      <c r="AM5" s="91"/>
+      <c r="AN5" s="91">
         <f>AG5+7</f>
         <v>44515</v>
       </c>
-      <c r="AO5" s="87"/>
-      <c r="AP5" s="87"/>
-      <c r="AQ5" s="87"/>
-      <c r="AR5" s="87"/>
-      <c r="AS5" s="87"/>
-      <c r="AT5" s="87"/>
-      <c r="AU5" s="87">
+      <c r="AO5" s="91"/>
+      <c r="AP5" s="91"/>
+      <c r="AQ5" s="91"/>
+      <c r="AR5" s="91"/>
+      <c r="AS5" s="91"/>
+      <c r="AT5" s="91"/>
+      <c r="AU5" s="91">
         <f>AN5+7</f>
         <v>44522</v>
       </c>
-      <c r="AV5" s="87"/>
-      <c r="AW5" s="87"/>
-      <c r="AX5" s="87"/>
-      <c r="AY5" s="87"/>
-      <c r="AZ5" s="87"/>
-      <c r="BA5" s="87"/>
-      <c r="BB5" s="88">
+      <c r="AV5" s="91"/>
+      <c r="AW5" s="91"/>
+      <c r="AX5" s="91"/>
+      <c r="AY5" s="91"/>
+      <c r="AZ5" s="91"/>
+      <c r="BA5" s="91"/>
+      <c r="BB5" s="95">
         <f>AU5+7</f>
         <v>44529</v>
       </c>
-      <c r="BC5" s="88"/>
-      <c r="BD5" s="88"/>
-      <c r="BE5" s="88"/>
-      <c r="BF5" s="88"/>
-      <c r="BG5" s="88"/>
-      <c r="BH5" s="88"/>
+      <c r="BC5" s="95"/>
+      <c r="BD5" s="95"/>
+      <c r="BE5" s="95"/>
+      <c r="BF5" s="95"/>
+      <c r="BG5" s="95"/>
+      <c r="BH5" s="95"/>
       <c r="BI5" s="9"/>
       <c r="BJ5" s="9"/>
       <c r="BK5" s="9"/>
@@ -4673,58 +4682,58 @@
       <c r="BZ5" s="9"/>
     </row>
     <row r="6" spans="1:78" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="90" t="s">
+      <c r="A6" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="90" t="s">
+      <c r="E6" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="F6" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="89" t="s">
+      <c r="G6" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="91" t="s">
+      <c r="I6" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="92" t="s">
+      <c r="J6" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="92" t="s">
+      <c r="K6" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="92" t="s">
+      <c r="L6" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="92" t="s">
+      <c r="M6" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="91" t="s">
+      <c r="N6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="91" t="s">
+      <c r="O6" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="92" t="s">
+      <c r="P6" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="97" t="s">
+      <c r="Q6" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="92" t="s">
+      <c r="R6" s="89" t="s">
         <v>47</v>
       </c>
       <c r="S6" s="4">
@@ -4897,24 +4906,24 @@
       </c>
     </row>
     <row r="7" spans="1:78" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="94"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="95"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="90"/>
       <c r="S7" s="6" t="str">
         <f t="shared" ref="S7:AX7" si="6">UPPER(LEFT(TEXT(S6,"ddd"),1))</f>
         <v>M</v>
@@ -7376,7 +7385,9 @@
       <c r="D22" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="E22" s="53"/>
+      <c r="E22" s="53" t="s">
+        <v>204</v>
+      </c>
       <c r="F22" s="66">
         <v>10</v>
       </c>
@@ -7465,7 +7476,9 @@
       <c r="D23" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="E23" s="53"/>
+      <c r="E23" s="53" t="s">
+        <v>205</v>
+      </c>
       <c r="F23" s="66">
         <v>10</v>
       </c>
@@ -9348,10 +9361,18 @@
       <c r="A36" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="53"/>
+      <c r="B36" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>206</v>
+      </c>
       <c r="F36" s="66"/>
       <c r="G36" s="74" t="s">
         <v>105</v>
@@ -25624,14 +25645,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="Z5:AF5"/>
-    <mergeCell ref="AG5:AM5"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="P6:P7"/>
     <mergeCell ref="AN5:AT5"/>
     <mergeCell ref="AU5:BA5"/>
     <mergeCell ref="BB5:BH5"/>
@@ -25648,6 +25661,14 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="Z5:AF5"/>
+    <mergeCell ref="AG5:AM5"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="P6:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:A14 L10:P11 L8:BH9 R10:BH11 A18 A23:A24 A37:A38 D27:F27 A45 D40:F45 H40:J45 L47:BH50 A54:A117 D47:F48 D54:J117 D50:F50 H47:J48 D49:J49 H50:J50 L52:BH117 D52:F53 H52:J53 D8:J26 H27:J28 D35:J39 E28:F28 L12:BH28 H31:J34 D31:F34 L31:BH45 E30">
     <cfRule type="expression" dxfId="188" priority="75" stopIfTrue="1">

</xml_diff>